<commit_message>
Readme and avg spender changes
</commit_message>
<xml_diff>
--- a/Project3/Q4/TopTenConsumers.xlsx
+++ b/Project3/Q4/TopTenConsumers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mystelvric/Documents/Mcgill/Winter 2018/421/Assignment/421DBProject1/Project3/Q4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD957FA-125D-F648-8030-C27C9EB115B1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDD192EA-1B97-D944-BFAB-2DDD9E128F93}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -141,7 +141,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="fr-FR" baseline="0"/>
-              <a:t> showing top 10 clients spenders in the year 2001</a:t>
+              <a:t> showing top 10 clients average spending in the year 2001</a:t>
             </a:r>
             <a:endParaRPr lang="fr-FR"/>
           </a:p>
@@ -203,10 +203,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="1">
                   <c:v>24</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>13</c:v>
@@ -242,10 +242,10 @@
                 <c:formatCode>_("$"* #,##0.00_);_("$"* \(#,##0.00\);_("$"* "-"??_);_(@_)</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>612</c:v>
+                  <c:v>521.73</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>521.73</c:v>
+                  <c:v>415.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>324.45</c:v>
@@ -1418,7 +1418,7 @@
   <dimension ref="A1:B13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1437,18 +1437,18 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2">
-        <v>612</v>
+        <v>521.73</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B3" s="2">
-        <v>521.73</v>
+        <v>415.82</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">

</xml_diff>